<commit_message>
Update hxl.input.info() for HXL-69
</commit_message>
<xml_diff>
--- a/tests/files/test_io/input-quality.xlsx
+++ b/tests/files/test_io/input-quality.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input-quality-no-hxl" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+  <si>
+    <t xml:space="preserve">¿Qué?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Quien?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Para quién?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Dónde?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Cuándo?</t>
+  </si>
   <si>
     <t xml:space="preserve">Registro</t>
   </si>
@@ -223,13 +238,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -265,15 +284,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
@@ -282,149 +301,174 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="H3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>105</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>110</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3"/>
       <c r="E4" s="0" t="n">
-        <v>250</v>
+        <v>105</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>110</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="0" t="n">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>28</v>
+        <v>300</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="D3:D4"/>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -441,15 +485,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
@@ -458,178 +502,199 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>13</v>
+      <c r="E3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="H4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>105</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>110</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" s="0" t="n">
-        <v>250</v>
+        <v>105</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="G5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>28</v>
+        <v>300</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug getting info for non-HXL CSV and JSON sources
</commit_message>
<xml_diff>
--- a/tests/files/test_io/input-quality.xlsx
+++ b/tests/files/test_io/input-quality.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="input-quality-no-hxl" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">¿Qué?</t>
   </si>
   <si>
-    <t xml:space="preserve">¿Quien?</t>
+    <t xml:space="preserve">¿Quién?</t>
   </si>
   <si>
     <t xml:space="preserve">¿Para quién?</t>
@@ -238,7 +238,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,16 +247,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -286,20 +290,19 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
+      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
@@ -487,20 +490,19 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="30.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.65"/>
@@ -508,22 +510,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -555,29 +557,29 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -606,7 +608,7 @@
       <c r="H4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -635,7 +637,7 @@
       <c r="H5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -664,7 +666,7 @@
       <c r="H6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -693,7 +695,7 @@
       <c r="H7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>